<commit_message>
Casos Pais  - parte cierre 17/4
</commit_message>
<xml_diff>
--- a/data/COVID-19.xlsx
+++ b/data/COVID-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eloy\Desktop\COVID 19\Dashboard\dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EDF5BF-4B8C-4F80-9772-14852F8BACF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3710D339-A437-4FD1-B89E-5666DD8DDC98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="749" activeTab="4" xr2:uid="{F2F8A79C-4094-4CDC-8A22-3CBB06EFC674}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="749" firstSheet="2" activeTab="7" xr2:uid="{F2F8A79C-4094-4CDC-8A22-3CBB06EFC674}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="14" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="192">
   <si>
     <t>Fecha</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>Baire</t>
+  </si>
+  <si>
+    <t>Día 38</t>
   </si>
 </sst>
 </file>
@@ -2213,15 +2216,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228926ED-9DEC-4DA3-841B-7744EBCE86DD}">
-  <dimension ref="A1:AK4"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AK6" sqref="AK6"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -2333,8 +2336,11 @@
       <c r="AK1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL1" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2446,13 +2452,16 @@
       <c r="AK2">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:AK3" si="0">SUM(A3,B2)</f>
+        <f t="shared" ref="B3:AL3" si="0">SUM(A3,B2)</f>
         <v>0</v>
       </c>
       <c r="C3">
@@ -2595,8 +2604,12 @@
         <f t="shared" si="0"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL3" s="20">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43901</v>
       </c>
@@ -2707,6 +2720,9 @@
       </c>
       <c r="AK4" s="2">
         <v>43937</v>
+      </c>
+      <c r="AL4" s="2">
+        <v>43938</v>
       </c>
     </row>
   </sheetData>
@@ -8212,7 +8228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437E6C5D-77A2-49DB-A15A-4AEFF9C341D7}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -11510,9 +11526,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BC42DC-9BE2-4B28-A5C7-CFAC0465C9D3}">
   <dimension ref="A1:AO20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AN18" sqref="AN18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO18" sqref="AO18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11522,7 +11538,7 @@
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -11643,8 +11659,11 @@
       <c r="AN1" s="20" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO1" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -11763,8 +11782,11 @@
       <c r="AN2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO2" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -11883,8 +11905,11 @@
       <c r="AN3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -12003,8 +12028,11 @@
       <c r="AN4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO4" s="20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -12123,8 +12151,11 @@
       <c r="AN5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO5" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -12243,8 +12274,11 @@
       <c r="AN6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO6" s="20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -12363,8 +12397,11 @@
       <c r="AN7">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO7" s="20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -12483,8 +12520,11 @@
       <c r="AN8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO8" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -12603,8 +12643,11 @@
       <c r="AN9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO9" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -12723,8 +12766,11 @@
       <c r="AN10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO10" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -12843,8 +12889,11 @@
       <c r="AN11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO11" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -12963,8 +13012,11 @@
       <c r="AN12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO12" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -13083,8 +13135,11 @@
       <c r="AN13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO13" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -13203,8 +13258,11 @@
       <c r="AN14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO14" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -13323,8 +13381,11 @@
       <c r="AN15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO15" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -13442,6 +13503,9 @@
       </c>
       <c r="AN16">
         <v>2</v>
+      </c>
+      <c r="AO16" s="20">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
@@ -13563,6 +13627,9 @@
       <c r="AN17">
         <v>3</v>
       </c>
+      <c r="AO17" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -13716,6 +13783,10 @@
         <f t="shared" si="13"/>
         <v>61</v>
       </c>
+      <c r="AO18" s="20">
+        <f t="shared" ref="AO18" si="14">SUM(AO2:AO17)</f>
+        <v>63</v>
+      </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -13832,7 +13903,9 @@
       <c r="AN19" s="2">
         <v>43937</v>
       </c>
-      <c r="AO19" s="2"/>
+      <c r="AO19" s="2">
+        <v>43938</v>
+      </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -13850,144 +13923,148 @@
         <v>4</v>
       </c>
       <c r="F20">
-        <f t="shared" ref="F20:AC20" si="14">SUM(E20,F18)</f>
+        <f t="shared" ref="F20:AC20" si="15">SUM(E20,F18)</f>
         <v>4</v>
       </c>
       <c r="G20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="H20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="I20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>10</v>
       </c>
       <c r="K20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
       <c r="L20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>16</v>
       </c>
       <c r="M20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>25</v>
       </c>
       <c r="N20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>35</v>
       </c>
       <c r="O20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>40</v>
       </c>
       <c r="P20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>48</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>57</v>
       </c>
       <c r="R20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>67</v>
       </c>
       <c r="S20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>80</v>
       </c>
       <c r="T20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>119</v>
       </c>
       <c r="U20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>139</v>
       </c>
       <c r="V20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>170</v>
       </c>
       <c r="W20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>186</v>
       </c>
       <c r="X20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>212</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>233</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>269</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>288</v>
       </c>
       <c r="AB20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>320</v>
       </c>
       <c r="AC20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>350</v>
       </c>
       <c r="AD20">
-        <f t="shared" ref="AD20" si="15">SUM(AC20,AD18)</f>
+        <f t="shared" ref="AD20" si="16">SUM(AC20,AD18)</f>
         <v>396</v>
       </c>
       <c r="AE20">
-        <f t="shared" ref="AE20" si="16">SUM(AD20,AE18)</f>
+        <f t="shared" ref="AE20" si="17">SUM(AD20,AE18)</f>
         <v>457</v>
       </c>
       <c r="AF20">
-        <f t="shared" ref="AF20:AG20" si="17">SUM(AE20,AF18)</f>
+        <f t="shared" ref="AF20:AG20" si="18">SUM(AE20,AF18)</f>
         <v>515</v>
       </c>
       <c r="AG20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>564</v>
       </c>
       <c r="AH20">
-        <f t="shared" ref="AH20" si="18">SUM(AG20,AH18)</f>
+        <f t="shared" ref="AH20" si="19">SUM(AG20,AH18)</f>
         <v>620</v>
       </c>
       <c r="AI20">
-        <f t="shared" ref="AI20" si="19">SUM(AH20,AI18)</f>
+        <f t="shared" ref="AI20" si="20">SUM(AH20,AI18)</f>
         <v>669</v>
       </c>
       <c r="AJ20">
-        <f t="shared" ref="AJ20" si="20">SUM(AI20,AJ18)</f>
+        <f t="shared" ref="AJ20" si="21">SUM(AI20,AJ18)</f>
         <v>726</v>
       </c>
       <c r="AK20">
-        <f t="shared" ref="AK20" si="21">SUM(AJ20,AK18)</f>
+        <f t="shared" ref="AK20" si="22">SUM(AJ20,AK18)</f>
         <v>766</v>
       </c>
       <c r="AL20">
-        <f t="shared" ref="AL20" si="22">SUM(AK20,AL18)</f>
+        <f t="shared" ref="AL20" si="23">SUM(AK20,AL18)</f>
         <v>814</v>
       </c>
       <c r="AM20">
-        <f t="shared" ref="AM20:AN20" si="23">SUM(AL20,AM18)</f>
+        <f t="shared" ref="AM20:AO20" si="24">SUM(AL20,AM18)</f>
         <v>862</v>
       </c>
       <c r="AN20" s="20">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>923</v>
+      </c>
+      <c r="AO20" s="20">
+        <f t="shared" si="24"/>
+        <v>986</v>
       </c>
     </row>
   </sheetData>
@@ -14001,8 +14078,8 @@
   <dimension ref="A1:AN20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD14" sqref="AD14"/>
+      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM1" sqref="AM1:AN20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14012,7 +14089,7 @@
     <col min="27" max="27" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -14130,8 +14207,11 @@
       <c r="AM1" s="20" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN1" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -14285,8 +14365,12 @@
         <f>IF(EXACT('Por Provincias'!AN2,""),"",SUM('Por Provincias'!AN2,Evolucion!AL2))</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN2" s="20">
+        <f>IF(EXACT('Por Provincias'!AO2,""),"",SUM('Por Provincias'!AO2,Evolucion!AM2))</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -14441,8 +14525,12 @@
         <f>IF(EXACT('Por Provincias'!AN3,""),"",SUM('Por Provincias'!AN3,Evolucion!AL3))</f>
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN3" s="20">
+        <f>IF(EXACT('Por Provincias'!AO3,""),"",SUM('Por Provincias'!AO3,Evolucion!AM3))</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -14592,8 +14680,12 @@
         <f>IF(EXACT('Por Provincias'!AN4,""),"",SUM('Por Provincias'!AN4,Evolucion!AL4))</f>
         <v>336</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN4" s="20">
+        <f>IF(EXACT('Por Provincias'!AO4,""),"",SUM('Por Provincias'!AO4,Evolucion!AM4))</f>
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>147</v>
       </c>
@@ -14726,8 +14818,12 @@
         <f>IF(EXACT('Por Provincias'!AN5,""),"",SUM('Por Provincias'!AN5,Evolucion!AL5))</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN5" s="20">
+        <f>IF(EXACT('Por Provincias'!AO5,""),"",SUM('Por Provincias'!AO5,Evolucion!AM5))</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>148</v>
       </c>
@@ -14878,8 +14974,12 @@
         <f>IF(EXACT('Por Provincias'!AN6,""),"",SUM('Por Provincias'!AN6,Evolucion!AL6))</f>
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN6" s="20">
+        <f>IF(EXACT('Por Provincias'!AO6,""),"",SUM('Por Provincias'!AO6,Evolucion!AM6))</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -15034,8 +15134,12 @@
         <f>IF(EXACT('Por Provincias'!AN7,""),"",SUM('Por Provincias'!AN7,Evolucion!AL7))</f>
         <v>145</v>
       </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN7" s="20">
+        <f>IF(EXACT('Por Provincias'!AO7,""),"",SUM('Por Provincias'!AO7,Evolucion!AM7))</f>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -15186,8 +15290,12 @@
         <f>IF(EXACT('Por Provincias'!AN8,""),"",SUM('Por Provincias'!AN8,Evolucion!AL8))</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN8" s="20">
+        <f>IF(EXACT('Por Provincias'!AO8,""),"",SUM('Por Provincias'!AO8,Evolucion!AM8))</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>183</v>
       </c>
@@ -15342,8 +15450,12 @@
         <f>IF(EXACT('Por Provincias'!AN9,""),"",SUM('Por Provincias'!AN9,Evolucion!AL9))</f>
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN9" s="20">
+        <f>IF(EXACT('Por Provincias'!AO9,""),"",SUM('Por Provincias'!AO9,Evolucion!AM9))</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>184</v>
       </c>
@@ -15486,8 +15598,12 @@
         <f>IF(EXACT('Por Provincias'!AN10,""),"",SUM('Por Provincias'!AN10,Evolucion!AL10))</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN10" s="20">
+        <f>IF(EXACT('Por Provincias'!AO10,""),"",SUM('Por Provincias'!AO10,Evolucion!AM10))</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -15642,8 +15758,12 @@
         <f>IF(EXACT('Por Provincias'!AN11,""),"",SUM('Por Provincias'!AN11,Evolucion!AL11))</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN11" s="20">
+        <f>IF(EXACT('Por Provincias'!AO11,""),"",SUM('Por Provincias'!AO11,Evolucion!AM11))</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -15791,8 +15911,12 @@
         <f>IF(EXACT('Por Provincias'!AN12,""),"",SUM('Por Provincias'!AN12,Evolucion!AL12))</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN12" s="20">
+        <f>IF(EXACT('Por Provincias'!AO12,""),"",SUM('Por Provincias'!AO12,Evolucion!AM12))</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -15940,8 +16064,12 @@
         <f>IF(EXACT('Por Provincias'!AN13,""),"",SUM('Por Provincias'!AN13,Evolucion!AL13))</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN13" s="20">
+        <f>IF(EXACT('Por Provincias'!AO13,""),"",SUM('Por Provincias'!AO13,Evolucion!AM13))</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -16088,8 +16216,12 @@
         <f>IF(EXACT('Por Provincias'!AN14,""),"",SUM('Por Provincias'!AN14,Evolucion!AL14))</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN14" s="20">
+        <f>IF(EXACT('Por Provincias'!AO14,""),"",SUM('Por Provincias'!AO14,Evolucion!AM14))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -16235,8 +16367,12 @@
         <f>IF(EXACT('Por Provincias'!AN15,""),"",SUM('Por Provincias'!AN15,Evolucion!AL15))</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN15" s="20">
+        <f>IF(EXACT('Por Provincias'!AO15,""),"",SUM('Por Provincias'!AO15,Evolucion!AM15))</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -16369,6 +16505,10 @@
         <f>IF(EXACT('Por Provincias'!AN16,""),"",SUM('Por Provincias'!AN16,Evolucion!AL16))</f>
         <v>13</v>
       </c>
+      <c r="AN16" s="20">
+        <f>IF(EXACT('Por Provincias'!AO16,""),"",SUM('Por Provincias'!AO16,Evolucion!AM16))</f>
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -16503,6 +16643,10 @@
         <f>IF(EXACT('Por Provincias'!AN17,""),"",SUM('Por Provincias'!AN17,Evolucion!AL17))</f>
         <v>20</v>
       </c>
+      <c r="AN17" s="20">
+        <f>IF(EXACT('Por Provincias'!AO17,""),"",SUM('Por Provincias'!AO17,Evolucion!AM17))</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -16656,6 +16800,10 @@
         <f>IF(EXACT('Por Provincias'!AN18,""),"",SUM('Por Provincias'!AN18,Evolucion!AL18))</f>
         <v>923</v>
       </c>
+      <c r="AN18" s="20">
+        <f>IF(EXACT('Por Provincias'!AO18,""),"",SUM('Por Provincias'!AO18,Evolucion!AM18))</f>
+        <v>986</v>
+      </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -16772,7 +16920,9 @@
       <c r="AM19" s="2">
         <v>43937</v>
       </c>
-      <c r="AN19" s="2"/>
+      <c r="AN19" s="2">
+        <v>43938</v>
+      </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -16923,8 +17073,12 @@
         <v>862</v>
       </c>
       <c r="AM20" s="20">
-        <f t="shared" ref="AM20" si="8">SUM(AM2:AM17)</f>
+        <f t="shared" ref="AM20:AN20" si="8">SUM(AM2:AM17)</f>
         <v>923</v>
+      </c>
+      <c r="AN20" s="20">
+        <f t="shared" si="8"/>
+        <v>986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>